<commit_message>
SPRINT 1: Improving team log and correting PDF document
</commit_message>
<xml_diff>
--- a/Documentation/Team Log.xlsx
+++ b/Documentation/Team Log.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\books\Concordia\LAST YEAR\SOEN 341\LuckySeven\Sprit 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\books\Concordia\LAST YEAR\SOEN 341\LuckySeven\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD33BFF4-C239-47C1-9B94-358571DFBB95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF82F00C-1C75-415B-A4F7-E1E04EF108D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="39">
   <si>
     <t>Task</t>
   </si>
@@ -88,6 +88,60 @@
   </si>
   <si>
     <t>Sprint 2</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>We have assigned the rules and responsibilities based on the previous experience of the team members and also based on individual interests.</t>
+  </si>
+  <si>
+    <t>Creating a GitHub repository and adding all Team members.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We have read the provided documents by the professor to have a general idea about the project. We have also discussed how we are going to approach the project and what technologies we were going to choose. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Summarizing all the discussed ideas in a well formated PDF. </t>
+  </si>
+  <si>
+    <t>User Stories</t>
+  </si>
+  <si>
+    <t>Writing all user stories based on the project description.</t>
+  </si>
+  <si>
+    <t>30mins</t>
+  </si>
+  <si>
+    <t>Creating the Wiki page</t>
+  </si>
+  <si>
+    <t>Creating a wiki page on GitHub and refrencing the excel planning sheet on it.</t>
+  </si>
+  <si>
+    <t>Kumai &amp; Yousef</t>
+  </si>
+  <si>
+    <t>Creating GitHub Issues</t>
+  </si>
+  <si>
+    <t>Youssef</t>
+  </si>
+  <si>
+    <t>Creating an issue for every task on the planning Excel Sheet.</t>
+  </si>
+  <si>
+    <t>Creating an Excel planning sheet</t>
+  </si>
+  <si>
+    <t>Creating a planning sheet to divide tasks and assign due dates. We had difficulties to plan for the next sprit because very minimum information were provided about sprint 2. The task has been assigned two days before the first sprint due date.</t>
+  </si>
+  <si>
+    <t>Having a team call to go over all the required documents and making sure nothing is missing</t>
+  </si>
+  <si>
+    <t>Writing the meeting minutes for most of the meetings</t>
   </si>
 </sst>
 </file>
@@ -210,32 +264,32 @@
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -517,115 +571,196 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="59.42578125" customWidth="1"/>
-    <col min="2" max="2" width="35" customWidth="1"/>
-    <col min="3" max="3" width="33.5703125" customWidth="1"/>
+    <col min="1" max="1" width="86.140625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="40.28515625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="35" style="3" customWidth="1"/>
+    <col min="4" max="4" width="33.5703125" style="3" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="5"/>
+    </row>
+    <row r="3" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="D3" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+    <row r="4" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="D4" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+    <row r="5" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="D6" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B7" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="D7" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="7" t="s">
+      <c r="B11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B12" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="D12" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+    <row r="13" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="4"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A13:D13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
working on update listing
</commit_message>
<xml_diff>
--- a/Documentation/Team Log.xlsx
+++ b/Documentation/Team Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriel Derhy\PhpstormProjects\LuckySeven\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69AA0855-A71F-44A0-B4C4-62EB216728F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21325072-81F4-4CF7-A3C3-CDD3C30A6B28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="48">
   <si>
     <t>Task</t>
   </si>
@@ -154,6 +154,21 @@
   </si>
   <si>
     <t>9h</t>
+  </si>
+  <si>
+    <t>Worked on turning the navbar into a reuseable component, and worked on the broker website</t>
+  </si>
+  <si>
+    <t>7h</t>
+  </si>
+  <si>
+    <t>Steven Zrihen</t>
+  </si>
+  <si>
+    <t>15hr</t>
+  </si>
+  <si>
+    <t>Worked on home page (indedx) , listings page, nav bar, the broker page, the functionality with a calandar on the broker page, the HTMLa dn CSS of these pages, the search page, implimented a slideshow function on the homepage (javascript), added a details page for each listing with a calculator functionality for the listings, HTML and CSS of the Login page. Contact and about-us page</t>
   </si>
 </sst>
 </file>
@@ -583,10 +598,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -783,6 +798,34 @@
         <v>42</v>
       </c>
     </row>
+    <row r="15" spans="1:5" ht="57" x14ac:dyDescent="0.45">
+      <c r="A15" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A16" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A2:D2"/>

</xml_diff>

<commit_message>
Filling up TeamLog - Kumai
</commit_message>
<xml_diff>
--- a/Documentation/Team Log.xlsx
+++ b/Documentation/Team Log.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriel Derhy\PhpstormProjects\LuckySeven\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\luckyseven\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21325072-81F4-4CF7-A3C3-CDD3C30A6B28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{491CAD31-5D04-4751-B3FF-B9DA07DCF0BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="60">
   <si>
     <t>Task</t>
   </si>
@@ -156,12 +156,6 @@
     <t>9h</t>
   </si>
   <si>
-    <t>Worked on turning the navbar into a reuseable component, and worked on the broker website</t>
-  </si>
-  <si>
-    <t>7h</t>
-  </si>
-  <si>
     <t>Steven Zrihen</t>
   </si>
   <si>
@@ -169,6 +163,48 @@
   </si>
   <si>
     <t>Worked on home page (indedx) , listings page, nav bar, the broker page, the functionality with a calandar on the broker page, the HTMLa dn CSS of these pages, the search page, implimented a slideshow function on the homepage (javascript), added a details page for each listing with a calculator functionality for the listings, HTML and CSS of the Login page. Contact and about-us page</t>
+  </si>
+  <si>
+    <t>Creating Sql querries and associated JavaScript functions for frontend-backend communications</t>
+  </si>
+  <si>
+    <t>I had communicated with Gabriel and Yousef to make sure the needed data, filer parameters, and all database related functions are available for the pages development.</t>
+  </si>
+  <si>
+    <t>8h</t>
+  </si>
+  <si>
+    <t>Working on the property search front-end back-end integration and improving UI</t>
+  </si>
+  <si>
+    <t>There are still work to be done to improve the user interface. For now, the user can easily search for properties by the area, maximum price, and if it is for sale or for rent.</t>
+  </si>
+  <si>
+    <t>5h</t>
+  </si>
+  <si>
+    <t>Steven and Kumai</t>
+  </si>
+  <si>
+    <t>Initializing CI/CD Pipeline on GitHub and making a basic testing architecture for the project</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It is difficult to perform test cases when the whole project is locally hosted. The test cases are done locally and the work perfectly. However, they do not work on GitHub since there is no way to connect to the local database. Hence, I have setup hard coded data for now, but this can be easily changed once a better database enviornment is set. </t>
+  </si>
+  <si>
+    <t>Setting up test cases for the project</t>
+  </si>
+  <si>
+    <t>There is only one php file to be tested. Other files are all JavaScript files. However, there are too many sql querries related functions that need to be tested.</t>
+  </si>
+  <si>
+    <t>Peer reviewing and support</t>
+  </si>
+  <si>
+    <t>6h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Helping other teams with the setup and debugging. </t>
   </si>
 </sst>
 </file>
@@ -598,22 +634,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="86.1328125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="40.265625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="86.140625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="40.28515625" style="3" customWidth="1"/>
     <col min="3" max="3" width="35" style="3" customWidth="1"/>
-    <col min="4" max="4" width="33.59765625" style="3" customWidth="1"/>
-    <col min="5" max="16384" width="9.1328125" style="3"/>
+    <col min="4" max="4" width="33.5703125" style="3" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -627,7 +663,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>19</v>
       </c>
@@ -636,7 +672,7 @@
       <c r="D2" s="6"/>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:5" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -650,7 +686,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
@@ -664,7 +700,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>26</v>
       </c>
@@ -678,7 +714,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -692,7 +728,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>12</v>
       </c>
@@ -706,7 +742,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>32</v>
       </c>
@@ -720,7 +756,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>29</v>
       </c>
@@ -734,7 +770,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>35</v>
       </c>
@@ -748,7 +784,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
@@ -762,7 +798,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>16</v>
       </c>
@@ -776,7 +812,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="18" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>20</v>
       </c>
@@ -784,7 +820,7 @@
       <c r="C13" s="8"/>
       <c r="D13" s="9"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>39</v>
       </c>
@@ -798,32 +834,88 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="57" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>40</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D15" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A16" s="5" t="s">
-        <v>43</v>
-      </c>
       <c r="B16" s="5" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="C16" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D16" s="5" t="s">
-        <v>44</v>
+      <c r="D17" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="135" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finalizing Sprint 3 documentation (Team Log + Planning sheet)
</commit_message>
<xml_diff>
--- a/Documentation/Team Log.xlsx
+++ b/Documentation/Team Log.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriel Derhy\PhpstormProjects\LuckySeven\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\luckyseven\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{016A5AFD-3D67-49AF-B384-DD5829F0FB99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{165A84EE-32C6-4CA7-AFE3-1EEEFEA6BCDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="80">
   <si>
     <t>Task</t>
   </si>
@@ -234,17 +234,44 @@
     <t>Sprint 3</t>
   </si>
   <si>
-    <t>Find brokers page, making a navbar component</t>
-  </si>
-  <si>
     <t>Gabriel and Kumai and Steven</t>
+  </si>
+  <si>
+    <t>Acceptance tests</t>
+  </si>
+  <si>
+    <t>wrote 6 acceptance tests</t>
+  </si>
+  <si>
+    <t>wrote 3 user strories for sprint 4 features (admin, broker, client)</t>
+  </si>
+  <si>
+    <t>This part was a bit tricky since we needed to link the offers table, the property tables, and the user table together</t>
+  </si>
+  <si>
+    <t>3h</t>
+  </si>
+  <si>
+    <t>Giving support and finalizing sprint 3</t>
+  </si>
+  <si>
+    <t>Reviewing user stories and acceptance tests. Making the wiki page and validating delieverable requirements</t>
+  </si>
+  <si>
+    <t>Working on the offer management page</t>
+  </si>
+  <si>
+    <t>Find brokers page, making a navbar component, offer submission</t>
+  </si>
+  <si>
+    <t>Implementing the needed functionalities to read the submitted and received offers</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -269,6 +296,12 @@
     </font>
     <font>
       <sz val="14"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -667,22 +700,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B18" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="86.1328125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="40.265625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="86.140625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="40.28515625" style="3" customWidth="1"/>
     <col min="3" max="3" width="35" style="3" customWidth="1"/>
-    <col min="4" max="4" width="33.59765625" style="3" customWidth="1"/>
-    <col min="5" max="16384" width="9.1328125" style="3"/>
+    <col min="4" max="4" width="33.5703125" style="3" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -696,7 +729,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>19</v>
       </c>
@@ -705,7 +738,7 @@
       <c r="D2" s="6"/>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:5" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -719,7 +752,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
@@ -733,7 +766,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>26</v>
       </c>
@@ -747,7 +780,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -761,7 +794,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>12</v>
       </c>
@@ -775,7 +808,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>32</v>
       </c>
@@ -789,7 +822,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>29</v>
       </c>
@@ -803,7 +836,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>35</v>
       </c>
@@ -817,7 +850,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
@@ -831,7 +864,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>16</v>
       </c>
@@ -845,7 +878,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="18" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>20</v>
       </c>
@@ -853,7 +886,7 @@
       <c r="C13" s="8"/>
       <c r="D13" s="9"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>39</v>
       </c>
@@ -867,7 +900,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="57" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>45</v>
       </c>
@@ -881,7 +914,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="57" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>46</v>
       </c>
@@ -895,7 +928,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>49</v>
       </c>
@@ -909,7 +942,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="114" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:4" ht="135" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>53</v>
       </c>
@@ -923,7 +956,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>55</v>
       </c>
@@ -937,7 +970,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>57</v>
       </c>
@@ -951,7 +984,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>60</v>
       </c>
@@ -965,7 +998,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>62</v>
       </c>
@@ -979,7 +1012,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>26</v>
       </c>
@@ -993,7 +1026,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>66</v>
       </c>
@@ -1007,7 +1040,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="18" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>68</v>
       </c>
@@ -1015,17 +1048,101 @@
       <c r="C25" s="8"/>
       <c r="D25" s="9"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>40</v>
       </c>
       <c r="C26" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="B28" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D32" s="5" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1035,6 +1152,7 @@
     <mergeCell ref="A13:D13"/>
     <mergeCell ref="A25:D25"/>
   </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>